<commit_message>
v1.0 - minimal script
</commit_message>
<xml_diff>
--- a/myntra_output_one.xlsx
+++ b/myntra_output_one.xlsx
@@ -448,12 +448,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>https://www.myntra.com/tshirts/adidas+originals/adidas-originals-women-typography-printed-v-neck-relaxed-fit-t-shirt/35713564/buy</t>
+          <t>https://www.myntra.com/saree/tikhi-imli/tikhi-imli-embellished-embroidered-net-saree/30711854/buy?utm_source=social_share_pdp&amp;utm_medium=deeplink&amp;utm_campaign=social_share_pdp_deeplink</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Seller: ADIDAS INDIA MARKETING PRIVATE LIMITED</t>
+          <t>Seller: Brand Baaja Bride - SJIT</t>
         </is>
       </c>
     </row>

</xml_diff>